<commit_message>
Restrict standards to ToL, MIxS, and DwC only
</commit_message>
<xml_diff>
--- a/dist/checklists/core/xlsx/dwc/sc_rnaseq_dwc_core.xlsx
+++ b/dist/checklists/core/xlsx/dwc/sc_rnaseq_dwc_core.xlsx
@@ -15,14 +15,17 @@
     <sheet name="Library Preparation" sheetId="6" r:id="rId6"/>
     <sheet name="Sequencing" sheetId="7" r:id="rId7"/>
     <sheet name="File" sheetId="8" r:id="rId8"/>
-    <sheet name="Raw Data Processing" sheetId="9" r:id="rId9"/>
+    <sheet name="Analysis Derived Data" sheetId="9" r:id="rId9"/>
+    <sheet name="Raw Data Processing" sheetId="10" r:id="rId10"/>
+    <sheet name="Downstream Processing" sheetId="11" r:id="rId11"/>
+    <sheet name="Data Availability Checklist" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="498">
   <si>
     <t>Study ID</t>
   </si>
@@ -123,6 +126,12 @@
     <t>Scientific Name</t>
   </si>
   <si>
+    <t>Organism</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
     <t>Tissue</t>
   </si>
   <si>
@@ -138,12 +147,21 @@
     <t>Medium</t>
   </si>
   <si>
+    <t>Accession Number</t>
+  </si>
+  <si>
     <t>Behaviour</t>
   </si>
   <si>
     <t>Scientific Name (optional)</t>
   </si>
   <si>
+    <t>Organism (optional)</t>
+  </si>
+  <si>
+    <t>Strain (optional)</t>
+  </si>
+  <si>
     <t>Tissue (optional)</t>
   </si>
   <si>
@@ -159,6 +177,9 @@
     <t>Medium (optional)</t>
   </si>
   <si>
+    <t>Accession Number (optional)</t>
+  </si>
+  <si>
     <t>Behaviour (optional)</t>
   </si>
   <si>
@@ -174,6 +195,12 @@
     <t>e.g. Arenicola marina</t>
   </si>
   <si>
+    <t>An identifier of the strain of the organism, if applicable.</t>
+  </si>
+  <si>
+    <t>e.g. CCAP1119/17</t>
+  </si>
+  <si>
     <t>The type of tissue sampled for the study.</t>
   </si>
   <si>
@@ -204,6 +231,12 @@
     <t>e.g. Tissue culture</t>
   </si>
   <si>
+    <t>A unique alphanumeric reference or identifier assigned to the sample in the study related to NCBI Taxonomy.</t>
+  </si>
+  <si>
+    <t>e.g. accession123</t>
+  </si>
+  <si>
     <t>A description of the behaviour shown by the subject at the time the dwc:Occurrence was recorded.</t>
   </si>
   <si>
@@ -678,12 +711,42 @@
     <t>Library Preparation Kit Version</t>
   </si>
   <si>
+    <t>Amplification Method</t>
+  </si>
+  <si>
+    <t>cDNA Amplification Cycles</t>
+  </si>
+  <si>
     <t>Average Size Distribution</t>
   </si>
   <si>
+    <t>Library Construction Method</t>
+  </si>
+  <si>
+    <t>Input Molecule</t>
+  </si>
+  <si>
+    <t>Primer</t>
+  </si>
+  <si>
     <t>Primeness</t>
   </si>
   <si>
+    <t>End Bias</t>
+  </si>
+  <si>
+    <t>Library Strand</t>
+  </si>
+  <si>
+    <t>Spike In</t>
+  </si>
+  <si>
+    <t>Spike Type</t>
+  </si>
+  <si>
+    <t>Spike In Dilution Or Concentration</t>
+  </si>
+  <si>
     <t>i5 Index</t>
   </si>
   <si>
@@ -717,6 +780,27 @@
     <t>Average Size Distribution (optional)</t>
   </si>
   <si>
+    <t>Library Construction Method (optional)</t>
+  </si>
+  <si>
+    <t>Input Molecule (optional)</t>
+  </si>
+  <si>
+    <t>Primer (optional)</t>
+  </si>
+  <si>
+    <t>End Bias (optional)</t>
+  </si>
+  <si>
+    <t>Library Strand (optional)</t>
+  </si>
+  <si>
+    <t>Spike Type (optional)</t>
+  </si>
+  <si>
+    <t>Spike In Dilution Or Concentration (optional)</t>
+  </si>
+  <si>
     <t>Plate ID (optional)</t>
   </si>
   <si>
@@ -744,18 +828,78 @@
     <t>e.g. 2</t>
   </si>
   <si>
+    <t>The method used to amplify the Complementary DNA (cDNA).</t>
+  </si>
+  <si>
+    <t>e.g. PCR</t>
+  </si>
+  <si>
+    <t>The number of cycles used during the Complementary DNA (cDNA) amplification process.</t>
+  </si>
+  <si>
+    <t>e.g. 12</t>
+  </si>
+  <si>
     <t>The average length of RNA fragments in base pairs (BP) after library preparation, indicating the quality and suitability of the RNA for sequencing.</t>
   </si>
   <si>
     <t>e.g. 350</t>
   </si>
   <si>
+    <t>The library construction method (including version) that was used.</t>
+  </si>
+  <si>
+    <t>e.g. Smart-Seq2</t>
+  </si>
+  <si>
+    <t>The specific fraction of biological macromolecule from which the sequencing library is derived.</t>
+  </si>
+  <si>
+    <t>e.g. RNA</t>
+  </si>
+  <si>
+    <t>The type of primer used for reverse transcription. This allows users to identify content of the cDNA library input for mRNA.</t>
+  </si>
+  <si>
+    <t>e.g. Random</t>
+  </si>
+  <si>
     <t>The end from which the molecule was sequenced.</t>
   </si>
   <si>
     <t>e.g. 5'</t>
   </si>
   <si>
+    <t>The end bias of the library.</t>
+  </si>
+  <si>
+    <t>e.g. 3</t>
+  </si>
+  <si>
+    <t>The Complementary DNA (cDNA) strand of the library from which the reads derived from - sense (first), antisense (second), both or none.</t>
+  </si>
+  <si>
+    <t>e.g. Antisense</t>
+  </si>
+  <si>
+    <t>External RNA added to the sample as a control to assess technical variability and normalization in RNA-sequencing. State whether spike-in was used.</t>
+  </si>
+  <si>
+    <t>e.g. Yes</t>
+  </si>
+  <si>
+    <t>The specific type of external RNA used for spiking in, often indicating the source or nature of the control RNA.</t>
+  </si>
+  <si>
+    <t>e.g. Synthetic RNA</t>
+  </si>
+  <si>
+    <t>The final concentration or dilution (for commercial sets) of the spike in mix.</t>
+  </si>
+  <si>
+    <t>e.g. 1:1000</t>
+  </si>
+  <si>
     <t>Barcode sequence used on the i5 adapter during library preparation for identifying samples in multiplexed single-cell RNA-sequencing.</t>
   </si>
   <si>
@@ -831,15 +975,24 @@
     <t>Desired Reads Per Cell</t>
   </si>
   <si>
+    <t>UMI Barcode Read</t>
+  </si>
+  <si>
+    <t>UMI Barcode Offset</t>
+  </si>
+  <si>
+    <t>UMI Barcode Size</t>
+  </si>
+  <si>
+    <t>Cell Barcode Read</t>
+  </si>
+  <si>
     <t>Cell Barcode Offset</t>
   </si>
   <si>
     <t>Cell Barcode Size</t>
   </si>
   <si>
-    <t>Cell Barcode Read</t>
-  </si>
-  <si>
     <t>cDNA Read</t>
   </si>
   <si>
@@ -849,15 +1002,24 @@
     <t>cDNA Read Size</t>
   </si>
   <si>
+    <t>UMI Barcode Read (optional)</t>
+  </si>
+  <si>
+    <t>UMI Barcode Offset (optional)</t>
+  </si>
+  <si>
+    <t>UMI Barcode Size (optional)</t>
+  </si>
+  <si>
+    <t>Cell Barcode Read (optional)</t>
+  </si>
+  <si>
     <t>Cell Barcode Offset (optional)</t>
   </si>
   <si>
     <t>Cell Barcode Size (optional)</t>
   </si>
   <si>
-    <t>Cell Barcode Read (optional)</t>
-  </si>
-  <si>
     <t>cDNA Read Offset (optional)</t>
   </si>
   <si>
@@ -892,6 +1054,27 @@
   </si>
   <si>
     <t>e.g. 1000000</t>
+  </si>
+  <si>
+    <t>The type of read that contains the Unique Molecular Identifier (UMI) barcode.</t>
+  </si>
+  <si>
+    <t>e.g. index2</t>
+  </si>
+  <si>
+    <t>The offset in sequence of the Unique Molecular Identifier (UMI) identifying barcode.</t>
+  </si>
+  <si>
+    <t>e.g. 0</t>
+  </si>
+  <si>
+    <t>The size of the Unique Molecular Identifier (UMI) identifying barcode.</t>
+  </si>
+  <si>
+    <t>The type of read that contains the UMI barcode.</t>
+  </si>
+  <si>
+    <t>e.g. index1</t>
   </si>
   <si>
     <t>The offset in sequence of the cell identifying barcode.</t>
@@ -901,15 +1084,6 @@
 E.g. "0".</t>
   </si>
   <si>
-    <t>e.g. 0</t>
-  </si>
-  <si>
-    <t>The type of read that contains the UMI barcode.</t>
-  </si>
-  <si>
-    <t>e.g. index1</t>
-  </si>
-  <si>
     <t>The actual nucleotide sequence obtained from Complementary DNA (cDNA) during sequencing.</t>
   </si>
   <si>
@@ -995,9 +1169,64 @@
     <t>e.g. barcodes.tsv</t>
   </si>
   <si>
+    <t>File Derived From</t>
+  </si>
+  <si>
+    <t>Inferred Cell Type</t>
+  </si>
+  <si>
+    <t>Post Analysis Cell Well Quality</t>
+  </si>
+  <si>
+    <t>Other Derived Cell Attributes</t>
+  </si>
+  <si>
+    <t>File Derived From (optional)</t>
+  </si>
+  <si>
+    <t>Inferred Cell Type (optional)</t>
+  </si>
+  <si>
+    <t>Post Analysis Cell Well Quality (optional)</t>
+  </si>
+  <si>
+    <t>Other Derived Cell Attributes (optional)</t>
+  </si>
+  <si>
+    <t>The name of the file that was used to generate the analysis derived data.</t>
+  </si>
+  <si>
+    <t>e.g. file1_sequencing.json</t>
+  </si>
+  <si>
+    <t>Post analysis cell type or identity declaration based on expression profile or known gene function identified by the performer.</t>
+  </si>
+  <si>
+    <t>e.g. type II bipolar neuron</t>
+  </si>
+  <si>
+    <t>Performer defined measure of whether the read output
+from the cell was included in the sequencing analysis. For example, cells might be excluded if a threshold percentage of reads did not map to the genome or if pre-sequencing quality measures were not passed.</t>
+  </si>
+  <si>
+    <t>e.g. Passed</t>
+  </si>
+  <si>
+    <t>Any other cell level measurement or annotation as result of the analysis.</t>
+  </si>
+  <si>
+    <t>e.g. cluster</t>
+  </si>
+  <si>
     <t>Reference Genome</t>
   </si>
   <si>
+    <t>Genome Annotation</t>
+  </si>
+  <si>
+    <t>Annotation Filtering</t>
+  </si>
+  <si>
     <t>Genes vs Exons</t>
   </si>
   <si>
@@ -1028,9 +1257,24 @@
     <t>Predicted Doublet Rate QC</t>
   </si>
   <si>
+    <t>Individual Organism SNP Demultiplexing</t>
+  </si>
+  <si>
+    <t>UMIs/Barcode Distribution QC</t>
+  </si>
+  <si>
+    <t>Cell/Non-Cell Filtering Strategy</t>
+  </si>
+  <si>
     <t>Reference Genome (optional)</t>
   </si>
   <si>
+    <t>Genome Annotation (optional)</t>
+  </si>
+  <si>
+    <t>Annotation Filtering (optional)</t>
+  </si>
+  <si>
     <t>Genes vs Exons (optional)</t>
   </si>
   <si>
@@ -1061,12 +1305,33 @@
     <t>Predicted Doublet Rate QC (optional)</t>
   </si>
   <si>
+    <t>Individual Organism SNP Demultiplexing (optional)</t>
+  </si>
+  <si>
+    <t>UMIs/Barcode Distribution QC (optional)</t>
+  </si>
+  <si>
+    <t>Cell/Non-Cell Filtering Strategy (optional)</t>
+  </si>
+  <si>
     <t>Indicate version and include stable link to genome data (or attach genome fasta file).</t>
   </si>
   <si>
     <t>e.g. GRCh38, https://example.org/grch38.fa</t>
   </si>
   <si>
+    <t>Indicate version and include stable link. Also indicate if any modification to the original annotation has been applied (e.g. 3' UTR extension) and include modified annotation file employed in the analysis.</t>
+  </si>
+  <si>
+    <t>e.g. Ensembl v101, https://example.org/ensembl_v101.gtf</t>
+  </si>
+  <si>
+    <t>Indicate which features were filtered (i.e. protein coding, pseudo-genes, TCRs, etc.)</t>
+  </si>
+  <si>
+    <t>e.g. Filtered to include only protein-coding genes</t>
+  </si>
+  <si>
     <t>Quantification using whole gene intervals or exons.</t>
   </si>
   <si>
@@ -1085,9 +1350,6 @@
     <t>e.g. Cell Ranger 6.0.0</t>
   </si>
   <si>
-    <t>Statistics of the Reads or Unique Molecular Identifier (UMI).</t>
-  </si>
-  <si>
     <t>e.g. 80% reads mapped to reference</t>
   </si>
   <si>
@@ -1122,6 +1384,144 @@
   </si>
   <si>
     <t>e.g. Predicted doublet rate: 1.5%</t>
+  </si>
+  <si>
+    <t>If carried out, show SNP partitioning quality (e.g. SNP UMAP embedding or covariance matrix), algorithm used</t>
+  </si>
+  <si>
+    <t>e.g. SNP UMAP embedding using CellSNP</t>
+  </si>
+  <si>
+    <t>Show UMIs per barcode distribution and threshold applied</t>
+  </si>
+  <si>
+    <t>UMI threshold used to discriminate cells from non-cells. Description of algorithm (if any) and parameters used to determine cells/non-cells.</t>
+  </si>
+  <si>
+    <t>Clustering Algorithm and Version</t>
+  </si>
+  <si>
+    <t>Clustering Parameters</t>
+  </si>
+  <si>
+    <t>Integration/Batch Correction</t>
+  </si>
+  <si>
+    <t>Clustering Algorithm and Version (optional)</t>
+  </si>
+  <si>
+    <t>Clustering Parameters (optional)</t>
+  </si>
+  <si>
+    <t>Integration/Batch Correction (optional)</t>
+  </si>
+  <si>
+    <t>If compared/integrated with existing datasets</t>
+  </si>
+  <si>
+    <t>e.g. Louvain 0.8.0</t>
+  </si>
+  <si>
+    <t>e.g. Resolution: 0.6, K-nearest neighbors: 10</t>
+  </si>
+  <si>
+    <t>e.g. Harmony v1.0</t>
+  </si>
+  <si>
+    <t>Source Code</t>
+  </si>
+  <si>
+    <t>UMI Count Matrix</t>
+  </si>
+  <si>
+    <t>Ensembl IDs</t>
+  </si>
+  <si>
+    <t>Functional Gene Annotations</t>
+  </si>
+  <si>
+    <t>Protein Models</t>
+  </si>
+  <si>
+    <t>Cell Metadata</t>
+  </si>
+  <si>
+    <t>Cluster-Level Normalised Expression Tables</t>
+  </si>
+  <si>
+    <t>Other Resource Files</t>
+  </si>
+  <si>
+    <t>Source Code (optional)</t>
+  </si>
+  <si>
+    <t>UMI Count Matrix (optional)</t>
+  </si>
+  <si>
+    <t>Ensembl IDs (optional)</t>
+  </si>
+  <si>
+    <t>Functional Gene Annotations (optional)</t>
+  </si>
+  <si>
+    <t>Protein Models (optional)</t>
+  </si>
+  <si>
+    <t>Cell Metadata (optional)</t>
+  </si>
+  <si>
+    <t>Cluster-Level Normalised Expression Tables (optional)</t>
+  </si>
+  <si>
+    <t>Other Resource Files (optional)</t>
+  </si>
+  <si>
+    <t>If any newly developed code/software has been used in the processing and downstream analysis of the dataset.</t>
+  </si>
+  <si>
+    <t>e.g. Source code is hosted on GitHub and includes custom algorithms for UMI count normalization. The repository can be found at: https://github.com/user/umi-normalization.</t>
+  </si>
+  <si>
+    <t>Gene x cell matrix with UMI counts for each gene in each cell.</t>
+  </si>
+  <si>
+    <t>e.g. The UMI count matrix is stored in a CSV file with gene IDs as rows (e.g., ENSG00000139618) and cell barcodes as columns (e.g., Cell_001, Cell_002). The matrix file is available at: https://example.com/umi_count_matrix.csv.</t>
+  </si>
+  <si>
+    <t>Gene or transcript names should be listed as Ensembl (or other standardized ID), with gene short names in metadata.</t>
+  </si>
+  <si>
+    <t>e.g. The UMI count matrix includes genes identified by their Ensembl IDs, such as 'ENSG00000139618' for the BRCA1 gene. See the full list of Ensembl IDs in the metadata file.</t>
+  </si>
+  <si>
+    <t>Any functional annotation generated/used (gene names, GOs, structural domains, etc.).</t>
+  </si>
+  <si>
+    <t>e.g. Functional gene annotations, including Gene Ontology (GO) terms, are provided in the metadata. For example, the gene 'ENSG00000139618' (BRCA1) is annotated with the GO term 'GO:0003674' (DNA binding).</t>
+  </si>
+  <si>
+    <t>FASTA file with (or stable link to) the predicted proteins associated to genes in the UMI count matrix and matching IDs.</t>
+  </si>
+  <si>
+    <t>e.g. The protein sequences for genes are provided in a FASTA file available at: https://example.com/protein_models.fasta, where each protein sequence is linked to the corresponding gene ID.</t>
+  </si>
+  <si>
+    <t>Table mapping cell IDs to cluster/cell type/broad cell type annotations.</t>
+  </si>
+  <si>
+    <t>e.g. Cell metadata includes information such as cell type annotations ('Tumor', 'Normal') and experimental conditions ('Control', 'Treatment'). This data is available in a table at: https://example.com/cell_metadata.csv.</t>
+  </si>
+  <si>
+    <t>Expression tables that show normalised gene expression at the cluster or cell-type level.</t>
+  </si>
+  <si>
+    <t>e.g. Normalised gene expression data at the cluster level is provided in a tab-delimited text file. For example, gene 'ENSG00000139618' (BRCA1) has expression values for clusters: Cluster_1: 1200, Cluster_2: 900. The full expression table is available at: https://example.com/cluster_level_expression.csv.</t>
+  </si>
+  <si>
+    <t>Necessary to re-use and interpret the data. E.g. barcode information in complex, serial multiplexing protocols (clicktags).</t>
+  </si>
+  <si>
+    <t>e.g. Barcode information used in multiplexing protocols is provided in a separate file, which can be accessed at: https://example.com/barcode_data.csv.</t>
   </si>
 </sst>
 </file>
@@ -1662,393 +2062,442 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C5:C78"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="179.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="152.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="85.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="97.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="75.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="124" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="85.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:3">
-      <c r="C5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3">
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="3:3">
-      <c r="C7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3">
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="3:3">
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="3:3">
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="3:3">
-      <c r="C11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="3:3">
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3">
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3">
-      <c r="C14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3">
-      <c r="C15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3">
-      <c r="C16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3">
-      <c r="C20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3">
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3">
-      <c r="C22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3">
-      <c r="C23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3">
-      <c r="C24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3">
-      <c r="C25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3">
-      <c r="C26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3">
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3">
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3">
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3">
-      <c r="C30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3">
-      <c r="C31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3">
-      <c r="C32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3">
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3">
-      <c r="C34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3">
-      <c r="C35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3">
-      <c r="C36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3">
-      <c r="C37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3">
-      <c r="C38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3">
-      <c r="C39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3">
-      <c r="C40" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3">
-      <c r="C41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3">
-      <c r="C42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3">
-      <c r="C43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3">
-      <c r="C44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3">
-      <c r="C45" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3">
-      <c r="C46" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="3:3">
-      <c r="C47" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="3:3">
-      <c r="C48" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3">
-      <c r="C51" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3">
-      <c r="C52" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3">
-      <c r="C53" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3">
-      <c r="C54" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3">
-      <c r="C55" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3">
-      <c r="C56" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3">
-      <c r="C57" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3">
-      <c r="C58" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="59" spans="3:3">
-      <c r="C59" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3">
-      <c r="C60" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3">
-      <c r="C61" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3">
-      <c r="C62" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3">
-      <c r="C63" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3">
-      <c r="C64" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3">
-      <c r="C65" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3">
-      <c r="C66" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3">
-      <c r="C67" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3">
-      <c r="C68" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="69" spans="3:3">
-      <c r="C69" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="70" spans="3:3">
-      <c r="C70" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="3:3">
-      <c r="C71" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="3:3">
-      <c r="C72" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3">
-      <c r="C73" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="74" spans="3:3">
-      <c r="C74" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="75" spans="3:3">
-      <c r="C75" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="3:3">
-      <c r="C76" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="77" spans="3:3">
-      <c r="C77" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="78" spans="3:3">
-      <c r="C78" t="s">
-        <v>135</v>
-      </c>
+    <row r="1" spans="1:25">
+      <c r="A1" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A4:Y4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:Y4">
+    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+      <formula>NOT(ISERROR(A1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="16">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(B5, ROW(INDIRECT("1:"&amp;LEN(B5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(C5, ROW(INDIRECT("1:"&amp;LEN(C5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(D5, ROW(INDIRECT("1:"&amp;LEN(D5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(E5, ROW(INDIRECT("1:"&amp;LEN(E5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(F5, ROW(INDIRECT("1:"&amp;LEN(F5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(G5, ROW(INDIRECT("1:"&amp;LEN(G5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(H5, ROW(INDIRECT("1:"&amp;LEN(H5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(I5, ROW(INDIRECT("1:"&amp;LEN(I5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(J5, ROW(INDIRECT("1:"&amp;LEN(J5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(K5, ROW(INDIRECT("1:"&amp;LEN(K5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(L5, ROW(INDIRECT("1:"&amp;LEN(L5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(M5, ROW(INDIRECT("1:"&amp;LEN(M5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(N5, ROW(INDIRECT("1:"&amp;LEN(N5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(O5, ROW(INDIRECT("1:"&amp;LEN(O5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5:P1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(P5, ROW(INDIRECT("1:"&amp;LEN(P5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="41.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A4:C4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:C4">
+    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+      <formula>NOT(ISERROR(A1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(B5, ROW(INDIRECT("1:"&amp;LEN(B5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(C5, ROW(INDIRECT("1:"&amp;LEN(C5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -2056,92 +2505,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="183.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="100" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="88" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="154.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="198.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="152.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="187.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="191.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="135" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
-        <v>31</v>
+      <c r="A1" s="5" t="s">
+        <v>474</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>475</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>476</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>41</v>
+        <v>477</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>42</v>
+        <v>478</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>43</v>
+        <v>479</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>44</v>
+        <v>480</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>45</v>
+        <v>481</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>482</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>484</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
+        <v>486</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>488</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>490</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>492</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>58</v>
+        <v>494</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>60</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>483</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>485</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>487</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>489</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>55</v>
+        <v>491</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>57</v>
+        <v>493</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>59</v>
+        <v>495</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>61</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2166,27 +2615,602 @@
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1005">
-      <formula1>AND(LEN(B5)&gt;0, CODE(LEFT(B5,1))&gt;=65, CODE(LEFT(B5,1))&lt;=90, SUM(--ISNUMBER(FIND(MID(B5, ROW(INDIRECT("1:"&amp;LEN(B5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="C5:C1005">
-      <formula1>HiddenDropdowns!$C$5:$C$78</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="D5:D1005">
-      <formula1>"Air Dried,Dry Ice,Ethanol/Dry Ice Slurry,Lyophilised,Not Applicable,Not Collected,Not Provided,Other,Rnalater,Snap Frozen"</formula1>
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(B5, ROW(INDIRECT("1:"&amp;LEN(B5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(C5, ROW(INDIRECT("1:"&amp;LEN(C5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(D5, ROW(INDIRECT("1:"&amp;LEN(D5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(E5, ROW(INDIRECT("1:"&amp;LEN(E5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F1005">
-      <formula1>AND(ISNUMBER(F5+0), F5&gt;=-180, F5&lt;=180)</formula1>
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(F5, ROW(INDIRECT("1:"&amp;LEN(F5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(G5, ROW(INDIRECT("1:"&amp;LEN(G5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(H5, ROW(INDIRECT("1:"&amp;LEN(H5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="E5:E78"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:5">
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="5:5">
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="5:5">
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="5:5">
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="5:5">
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="5:5">
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="5:5">
+      <c r="E11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="5:5">
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="5:5">
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5">
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5">
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5">
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5">
+      <c r="E22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5">
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5">
+      <c r="E24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5">
+      <c r="E25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5">
+      <c r="E26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5">
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5">
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5">
+      <c r="E29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5">
+      <c r="E30" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5">
+      <c r="E31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5">
+      <c r="E32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="5:5">
+      <c r="E44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5">
+      <c r="E45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="5:5">
+      <c r="E46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5">
+      <c r="E47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="5:5">
+      <c r="E48" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5">
+      <c r="E51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5">
+      <c r="E52" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5">
+      <c r="E53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5">
+      <c r="E54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5">
+      <c r="E55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="5:5">
+      <c r="E56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5">
+      <c r="E57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5">
+      <c r="E58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="5:5">
+      <c r="E59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="5:5">
+      <c r="E60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="5:5">
+      <c r="E61" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5">
+      <c r="E62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="5:5">
+      <c r="E63" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="5:5">
+      <c r="E64" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5">
+      <c r="E65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5">
+      <c r="E66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="5:5">
+      <c r="E67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="5:5">
+      <c r="E68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="5:5">
+      <c r="E69" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" spans="5:5">
+      <c r="E70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="5:5">
+      <c r="E71" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="5:5">
+      <c r="E72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="5:5">
+      <c r="E73" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="5:5">
+      <c r="E74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="5:5">
+      <c r="E75" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="76" spans="5:5">
+      <c r="E76" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" spans="5:5">
+      <c r="E77" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="5:5">
+      <c r="E78" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="54.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="42" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="183.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="100" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="97.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="88" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A4:K4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:K4">
+    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+      <formula>NOT(ISERROR(A1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="10">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1005">
+      <formula1>AND(LEN(B5)&gt;0, CODE(LEFT(B5,1))&gt;=65, CODE(LEFT(B5,1))&lt;=90, SUM(--ISNUMBER(FIND(MID(B5, ROW(INDIRECT("1:"&amp;LEN(B5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1005">
+      <formula1>AND(LEN(C5)&gt;0, CODE(LEFT(C5,1))&gt;=65, CODE(LEFT(C5,1))&lt;=90, SUM(--ISNUMBER(FIND(MID(C5, ROW(INDIRECT("1:"&amp;LEN(C5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(D5, ROW(INDIRECT("1:"&amp;LEN(D5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="E5:E1005">
+      <formula1>HiddenDropdowns!$E$5:$E$78</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="F5:F1005">
+      <formula1>"Air Dried,Dry Ice,Ethanol/Dry Ice Slurry,Lyophilised,Not Applicable,Not Collected,Not Provided,Other,Rnalater,Snap Frozen"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H1005">
+      <formula1>AND(ISNUMBER(H5+0), H5&gt;=-180, H5&lt;=180)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(I5, ROW(INDIRECT("1:"&amp;LEN(I5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(J5, ROW(INDIRECT("1:"&amp;LEN(J5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(K5, ROW(INDIRECT("1:"&amp;LEN(K5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2215,98 +3239,98 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2397,122 +3421,122 @@
         <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2589,7 +3613,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2598,162 +3622,262 @@
     <col min="1" max="1" width="98.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="128" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="120" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="86.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="106.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="64.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="66.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="128" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="108.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="122" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="131.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="97.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="67.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="120" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="86.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="106.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="61.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="72.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="60.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="53" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="64.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="66.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:25">
       <c r="A1" s="2" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>225</v>
+        <v>234</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>232</v>
+        <v>255</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>257</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" s="3" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>289</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="3" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>290</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -2771,6 +3895,291 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A4:Y4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:Y4">
+    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+      <formula>NOT(ISERROR(A1))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="25">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(B5, ROW(INDIRECT("1:"&amp;LEN(B5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(C5, ROW(INDIRECT("1:"&amp;LEN(C5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(D5, ROW(INDIRECT("1:"&amp;LEN(D5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(E5, ROW(INDIRECT("1:"&amp;LEN(E5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(F5, ROW(INDIRECT("1:"&amp;LEN(F5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(G5, ROW(INDIRECT("1:"&amp;LEN(G5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(H5, ROW(INDIRECT("1:"&amp;LEN(H5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="I5:I1005">
+      <formula1>"Oligo-Dt,Random"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="J5:J1005">
+      <formula1>"3',5',Both"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="K5:K1005">
+      <formula1>"3,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="L5:L1005">
+      <formula1>"Antisense,Both,Sense,Unstranded"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="M5:M1005">
+      <formula1>"No,Yes"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(N5, ROW(INDIRECT("1:"&amp;LEN(N5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(O5, ROW(INDIRECT("1:"&amp;LEN(O5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5:P1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(P5, ROW(INDIRECT("1:"&amp;LEN(P5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q5:Q1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(Q5, ROW(INDIRECT("1:"&amp;LEN(Q5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="R5:R1005">
+      <formula1>"Dual,Single"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S5:S1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(S5, ROW(INDIRECT("1:"&amp;LEN(S5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(T5, ROW(INDIRECT("1:"&amp;LEN(T5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5:U1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(U5, ROW(INDIRECT("1:"&amp;LEN(U5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V5:V1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(V5, ROW(INDIRECT("1:"&amp;LEN(V5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W5:W1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(W5, ROW(INDIRECT("1:"&amp;LEN(W5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X5:X1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(X5, ROW(INDIRECT("1:"&amp;LEN(X5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="Y5:Y1005">
+      <formula1>"Cd41+,Cd41-"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="67.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="126.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="85.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="147.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2782,7 +4191,7 @@
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="15">
+  <dataValidations count="14">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
@@ -2792,230 +4201,38 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(C5, ROW(INDIRECT("1:"&amp;LEN(C5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(D5, ROW(INDIRECT("1:"&amp;LEN(D5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="E5:E1005">
-      <formula1>"3',5',Both"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(F5, ROW(INDIRECT("1:"&amp;LEN(F5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="D5:D1005">
+      <formula1>"Paired,Pool,Single"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E1005">
+      <formula1>AND(SUM(--ISNUMBER(FIND(MID(E5, ROW(INDIRECT("1:"&amp;LEN(E5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="F5:F1005">
+      <formula1>"Index1,Index2,Read1,Read2"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(G5, ROW(INDIRECT("1:"&amp;LEN(G5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="H5:H1005">
-      <formula1>"Dual,Single"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(I5, ROW(INDIRECT("1:"&amp;LEN(I5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+      <formula1>AND(ISNUMBER(G5+0), INT(G5+0)=G5+0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H1005">
+      <formula1>AND(ISNUMBER(H5+0), INT(H5+0)=H5+0)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="I5:I1005">
+      <formula1>"Index1,Index2,Read1,Read2"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(J5, ROW(INDIRECT("1:"&amp;LEN(J5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+      <formula1>AND(ISNUMBER(J5+0), INT(J5+0)=J5+0)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(K5, ROW(INDIRECT("1:"&amp;LEN(K5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(L5, ROW(INDIRECT("1:"&amp;LEN(L5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M5:M1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(M5, ROW(INDIRECT("1:"&amp;LEN(M5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+      <formula1>AND(ISNUMBER(K5+0), INT(K5+0)=K5+0)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="L5:L1005">
+      <formula1>"Index1,Index2,Read1,Read2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="M5:M1005">
+      <formula1>"Index1,Index2,Read1,Read2"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(N5, ROW(INDIRECT("1:"&amp;LEN(N5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="O5:O1005">
-      <formula1>"Cd41+,Cd41-"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="67.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="126.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="85.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="147.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="1">
-    <mergeCell ref="A4:K4"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A1:K4">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
-      <formula>NOT(ISERROR(A1))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="11">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(B5, ROW(INDIRECT("1:"&amp;LEN(B5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(C5, ROW(INDIRECT("1:"&amp;LEN(C5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="D5:D1005">
-      <formula1>"Paired,Pool,Single"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(E5, ROW(INDIRECT("1:"&amp;LEN(E5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F1005">
-      <formula1>AND(ISNUMBER(F5+0), INT(F5+0)=F5+0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G1005">
-      <formula1>AND(ISNUMBER(G5+0), INT(G5+0)=G5+0)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="H5:H1005">
-      <formula1>"Index1,Index2,Read1,Read2"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="I5:I1005">
-      <formula1>"Index1,Index2,Read1,Read2"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="J5:J1005">
-      <formula1>"Index1,Index2,Read1,Read2"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(K5, ROW(INDIRECT("1:"&amp;LEN(K5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3041,89 +4258,89 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>264</v>
+        <v>311</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>301</v>
+        <v>358</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>302</v>
+        <v>359</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>303</v>
+        <v>360</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>304</v>
+        <v>361</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>305</v>
+        <v>362</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>306</v>
+        <v>363</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>308</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>280</v>
+        <v>333</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>309</v>
+        <v>366</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>313</v>
+        <v>370</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>315</v>
+        <v>372</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>317</v>
+        <v>374</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>319</v>
+        <v>376</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>321</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>281</v>
+        <v>334</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>314</v>
+        <v>371</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>316</v>
+        <v>373</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>318</v>
+        <v>375</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>322</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3184,188 +4401,90 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="75.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="79.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="152.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="85.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="185.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
-        <v>334</v>
+        <v>384</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>335</v>
+        <v>385</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>336</v>
+        <v>386</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>345</v>
+        <v>388</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>347</v>
+        <v>390</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>349</v>
+        <v>392</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>346</v>
+        <v>389</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>348</v>
+        <v>391</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>350</v>
+        <v>393</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:K4">
+  <conditionalFormatting sqref="A1:D4">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="11">
+  <dataValidations count="4">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(B5, ROW(INDIRECT("1:"&amp;LEN(B5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(C5, ROW(INDIRECT("1:"&amp;LEN(C5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(D5, ROW(INDIRECT("1:"&amp;LEN(D5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(E5, ROW(INDIRECT("1:"&amp;LEN(E5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(F5, ROW(INDIRECT("1:"&amp;LEN(F5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(G5, ROW(INDIRECT("1:"&amp;LEN(G5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(H5, ROW(INDIRECT("1:"&amp;LEN(H5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(I5, ROW(INDIRECT("1:"&amp;LEN(I5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(J5, ROW(INDIRECT("1:"&amp;LEN(J5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(K5, ROW(INDIRECT("1:"&amp;LEN(K5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="C5:C1005">
+      <formula1>"Fail,Pass"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose from the list" sqref="D5:D1005">
+      <formula1>"Cluster,Count,Gene,Tsne Coordinates,Umi"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added additional mixs terms
</commit_message>
<xml_diff>
--- a/dist/checklists/core/xlsx/dwc/sc_rnaseq_dwc_core.xlsx
+++ b/dist/checklists/core/xlsx/dwc/sc_rnaseq_dwc_core.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="493">
   <si>
     <t>Study ID</t>
   </si>
@@ -1260,12 +1260,6 @@
     <t>Individual Organism SNP Demultiplexing</t>
   </si>
   <si>
-    <t>UMIs/Barcode Distribution QC</t>
-  </si>
-  <si>
-    <t>Cell/Non-Cell Filtering Strategy</t>
-  </si>
-  <si>
     <t>Reference Genome (optional)</t>
   </si>
   <si>
@@ -1308,12 +1302,6 @@
     <t>Individual Organism SNP Demultiplexing (optional)</t>
   </si>
   <si>
-    <t>UMIs/Barcode Distribution QC (optional)</t>
-  </si>
-  <si>
-    <t>Cell/Non-Cell Filtering Strategy (optional)</t>
-  </si>
-  <si>
     <t>Indicate version and include stable link to genome data (or attach genome fasta file).</t>
   </si>
   <si>
@@ -1350,6 +1338,9 @@
     <t>e.g. Cell Ranger 6.0.0</t>
   </si>
   <si>
+    <t>Statistics of the Reads or Unique Molecular Identifier (UMI).</t>
+  </si>
+  <si>
     <t>e.g. 80% reads mapped to reference</t>
   </si>
   <si>
@@ -1390,12 +1381,6 @@
   </si>
   <si>
     <t>e.g. SNP UMAP embedding using CellSNP</t>
-  </si>
-  <si>
-    <t>Show UMIs per barcode distribution and threshold applied</t>
-  </si>
-  <si>
-    <t>UMI threshold used to discriminate cells from non-cells. Description of algorithm (if any) and parameters used to determine cells/non-cells.</t>
   </si>
   <si>
     <t>Clustering Algorithm and Version</t>
@@ -2064,7 +2049,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2076,7 +2061,7 @@
     <col min="4" max="4" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="79.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="152.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2084,251 +2069,141 @@
     <col min="12" max="12" width="85.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="97.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="75.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="124" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="66.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="85.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="63.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:14">
       <c r="A1" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>421</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="M1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="B2" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="V1" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="W1" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="A3" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -2345,29 +2220,18 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A4:Y4"/>
+    <mergeCell ref="A4:N4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:Y4">
+  <conditionalFormatting sqref="A1:N4">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="16">
+  <dataValidations count="14">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(A5, ROW(INDIRECT("1:"&amp;LEN(A5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
@@ -2409,12 +2273,6 @@
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N5:N1005">
       <formula1>AND(SUM(--ISNUMBER(FIND(MID(N5, ROW(INDIRECT("1:"&amp;LEN(N5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(O5, ROW(INDIRECT("1:"&amp;LEN(O5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P5:P1005">
-      <formula1>AND(SUM(--ISNUMBER(FIND(MID(P5, ROW(INDIRECT("1:"&amp;LEN(P5))), 1), "abcdefghijklmnopqrstuvwxyz"))) &gt; 0)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2434,35 +2292,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2517,80 +2375,80 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>476</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3999,7 +3857,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4015,13 +3873,12 @@
     <col min="8" max="8" width="62.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="85.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="147.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="85.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="147.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>311</v>
       </c>
@@ -4055,20 +3912,17 @@
       <c r="K1" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>322</v>
       </c>
+      <c r="M1" s="5" t="s">
+        <v>331</v>
+      </c>
       <c r="N1" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="O1" s="5" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:14">
       <c r="A2" s="3" t="s">
         <v>333</v>
       </c>
@@ -4103,19 +3957,16 @@
         <v>351</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="O2" s="3" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
         <v>334</v>
       </c>
@@ -4150,19 +4001,16 @@
         <v>346</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="O3" s="3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -4179,14 +4027,13 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A4:N4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:O4">
+  <conditionalFormatting sqref="A1:N4">
     <cfRule type="notContainsErrors" dxfId="0" priority="1">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>

</xml_diff>